<commit_message>
Chore: all excercises complete
</commit_message>
<xml_diff>
--- a/2 Formulas and Functions/Formulas and Functions - 1. Basic Formulas and Functions.xlsx
+++ b/2 Formulas and Functions/Formulas and Functions - 1. Basic Formulas and Functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Analyst Builder\9.0 Excel for Data Analysis\4. Formulas and Functions\Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4879da3f5c650214/Desktop/Excel-for-Data-Analysis/2 Formulas and Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C73AD2B7-7254-45BC-9216-F89BD3AC8FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{C73AD2B7-7254-45BC-9216-F89BD3AC8FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0C9D298-17D5-4B49-B879-68AA5EB3F7E7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -214,9 +214,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -519,13 +516,13 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="13.6640625" style="1"/>
-    <col min="4" max="4" width="13.6640625" style="14"/>
+    <col min="4" max="4" width="13.6640625" style="13"/>
     <col min="5" max="6" width="13.6640625" style="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="16.83203125" customWidth="1"/>
@@ -542,7 +539,7 @@
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -562,13 +559,16 @@
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>1200</v>
       </c>
       <c r="E2" s="4">
         <v>37</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7">
+        <f>PRODUCT(D2,E2)</f>
+        <v>44400</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
@@ -580,13 +580,16 @@
       <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>1000</v>
       </c>
       <c r="E3" s="4">
         <v>31</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7">
+        <f t="shared" ref="F3:F30" si="0">PRODUCT(D3,E3)</f>
+        <v>31000</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
@@ -598,23 +601,29 @@
       <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>5000</v>
       </c>
       <c r="E4" s="4">
         <v>10</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7">
+        <f t="shared" si="0"/>
+        <v>50000</v>
+      </c>
       <c r="H4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="8"/>
+      <c r="I4" s="8">
+        <f>COUNTIF(A:A, "&lt;&gt;") -1</f>
+        <v>29</v>
+      </c>
       <c r="J4" s="2"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>4536</v>
+        <v>1</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
@@ -622,13 +631,16 @@
       <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>5000</v>
       </c>
       <c r="E5" s="4">
         <v>18</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7">
+        <f t="shared" si="0"/>
+        <v>90000</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -644,17 +656,23 @@
       <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>1000</v>
       </c>
       <c r="E6" s="4">
         <v>24</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7">
+        <f t="shared" si="0"/>
+        <v>24000</v>
+      </c>
       <c r="H6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="8"/>
+      <c r="I6" s="8">
+        <f>SUM(E:E)</f>
+        <v>700</v>
+      </c>
       <c r="J6" s="2"/>
       <c r="K6" s="1"/>
     </row>
@@ -668,17 +686,23 @@
       <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>5000</v>
       </c>
       <c r="E7" s="4">
         <v>20</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
       <c r="H7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="9"/>
+      <c r="I7" s="9">
+        <f>SUM(F:F)</f>
+        <v>1462000</v>
+      </c>
       <c r="J7" s="2"/>
       <c r="K7" s="1"/>
     </row>
@@ -692,13 +716,16 @@
       <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>1200</v>
       </c>
       <c r="E8" s="4">
         <v>22</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7">
+        <f t="shared" si="0"/>
+        <v>26400</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="1"/>
       <c r="J8" s="2"/>
@@ -714,13 +741,16 @@
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>5000</v>
       </c>
       <c r="E9" s="4">
         <v>23</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7">
+        <f t="shared" si="0"/>
+        <v>115000</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="6" t="s">
         <v>8</v>
@@ -742,19 +772,31 @@
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <v>1200</v>
       </c>
       <c r="E10" s="4">
         <v>20</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7">
+        <f t="shared" si="0"/>
+        <v>24000</v>
+      </c>
       <c r="H10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="10"/>
+      <c r="I10" s="8">
+        <f>COUNTIF(C:C, H10)</f>
+        <v>13</v>
+      </c>
+      <c r="J10" s="8">
+        <f>SUMIF(C:C, H10, E:E)</f>
+        <v>348</v>
+      </c>
+      <c r="K10" s="8">
+        <f>SUMIF(C:C, H10, F:F)</f>
+        <v>348000</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
@@ -766,19 +808,31 @@
       <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>1000</v>
       </c>
       <c r="E11" s="4">
         <v>27</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7">
+        <f t="shared" si="0"/>
+        <v>27000</v>
+      </c>
       <c r="H11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="10"/>
+      <c r="I11" s="8">
+        <f t="shared" ref="I11:I12" si="1">COUNTIF(C:C, H11)</f>
+        <v>6</v>
+      </c>
+      <c r="J11" s="8">
+        <f t="shared" ref="J11:J12" si="2">SUMIF(C:C, H11, E:E)</f>
+        <v>170</v>
+      </c>
+      <c r="K11" s="8">
+        <f t="shared" ref="K11:K12" si="3">SUMIF(C:C, H11, F:F)</f>
+        <v>204000</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
@@ -790,19 +844,31 @@
       <c r="C12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <v>1000</v>
       </c>
       <c r="E12" s="4">
         <v>19</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7">
+        <f t="shared" si="0"/>
+        <v>19000</v>
+      </c>
       <c r="H12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="10"/>
+      <c r="I12" s="8">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J12" s="8">
+        <f t="shared" si="2"/>
+        <v>182</v>
+      </c>
+      <c r="K12" s="8">
+        <f t="shared" si="3"/>
+        <v>910000</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
@@ -814,13 +880,16 @@
       <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="11">
         <v>5000</v>
       </c>
       <c r="E13" s="4">
         <v>16</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="7">
+        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -836,13 +905,16 @@
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <v>1000</v>
       </c>
       <c r="E14" s="4">
         <v>30</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7">
+        <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="2"/>
       <c r="J14" s="1"/>
@@ -858,17 +930,23 @@
       <c r="C15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="11">
         <v>1200</v>
       </c>
       <c r="E15" s="4">
         <v>33</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7">
+        <f t="shared" si="0"/>
+        <v>39600</v>
+      </c>
       <c r="H15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="8"/>
+      <c r="I15" s="8">
+        <f>COUNT(_xlfn.UNIQUE(B:B))</f>
+        <v>29</v>
+      </c>
       <c r="J15" s="2"/>
       <c r="K15" s="1"/>
     </row>
@@ -882,13 +960,16 @@
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="11">
         <v>5000</v>
       </c>
       <c r="E16" s="4">
         <v>39</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7">
+        <f t="shared" si="0"/>
+        <v>195000</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
@@ -900,13 +981,16 @@
       <c r="C17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <v>1000</v>
       </c>
       <c r="E17" s="4">
         <v>38</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7">
+        <f t="shared" si="0"/>
+        <v>38000</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
@@ -918,13 +1002,16 @@
       <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="11">
         <v>1000</v>
       </c>
       <c r="E18" s="4">
         <v>11</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="7">
+        <f t="shared" si="0"/>
+        <v>11000</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
@@ -936,13 +1023,16 @@
       <c r="C19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="11">
         <v>1000</v>
       </c>
       <c r="E19" s="4">
         <v>24</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="7">
+        <f t="shared" si="0"/>
+        <v>24000</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
@@ -954,13 +1044,16 @@
       <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="11">
         <v>1200</v>
       </c>
       <c r="E20" s="4">
         <v>32</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="7">
+        <f t="shared" si="0"/>
+        <v>38400</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
@@ -972,13 +1065,16 @@
       <c r="C21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="11">
         <v>5000</v>
       </c>
       <c r="E21" s="4">
         <v>13</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="7">
+        <f t="shared" si="0"/>
+        <v>65000</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
@@ -990,13 +1086,16 @@
       <c r="C22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="11">
         <v>1000</v>
       </c>
       <c r="E22" s="4">
         <v>35</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="7">
+        <f t="shared" si="0"/>
+        <v>35000</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
@@ -1008,13 +1107,16 @@
       <c r="C23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="11">
         <v>1000</v>
       </c>
       <c r="E23" s="4">
         <v>12</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7">
+        <f t="shared" si="0"/>
+        <v>12000</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
@@ -1026,13 +1128,16 @@
       <c r="C24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="11">
         <v>1000</v>
       </c>
       <c r="E24" s="4">
         <v>35</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="7">
+        <f t="shared" si="0"/>
+        <v>35000</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
@@ -1044,13 +1149,16 @@
       <c r="C25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="11">
         <v>5000</v>
       </c>
       <c r="E25" s="4">
         <v>16</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7">
+        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
@@ -1062,13 +1170,16 @@
       <c r="C26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="11">
         <v>1000</v>
       </c>
       <c r="E26" s="4">
         <v>29</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="7">
+        <f t="shared" si="0"/>
+        <v>29000</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
@@ -1080,13 +1191,16 @@
       <c r="C27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="11">
         <v>1200</v>
       </c>
       <c r="E27" s="4">
         <v>26</v>
       </c>
-      <c r="F27" s="7"/>
+      <c r="F27" s="7">
+        <f t="shared" si="0"/>
+        <v>31200</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
@@ -1098,13 +1212,16 @@
       <c r="C28" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="11">
         <v>1000</v>
       </c>
       <c r="E28" s="4">
         <v>33</v>
       </c>
-      <c r="F28" s="7"/>
+      <c r="F28" s="7">
+        <f t="shared" si="0"/>
+        <v>33000</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
@@ -1116,13 +1233,16 @@
       <c r="C29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="11">
         <v>5000</v>
       </c>
       <c r="E29" s="4">
         <v>16</v>
       </c>
-      <c r="F29" s="7"/>
+      <c r="F29" s="7">
+        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
@@ -1134,16 +1254,19 @@
       <c r="C30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="11">
         <v>5000</v>
       </c>
       <c r="E30" s="4">
         <v>11</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7">
+        <f t="shared" si="0"/>
+        <v>55000</v>
+      </c>
     </row>
     <row r="45" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D45" s="13"/>
+      <c r="D45" s="12"/>
       <c r="E45" s="2"/>
     </row>
   </sheetData>

</xml_diff>